<commit_message>
Agregando los datos de los estudiantes en el excel
</commit_message>
<xml_diff>
--- a/Colegio.xlsx
+++ b/Colegio.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26922394e5d0c289/Desktop/preParcial/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4D2F04E46CFB4ACB3E209D9595F0AC683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A46FA276-EF18-466F-A269-AE8A32E0D6B3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,82 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+  <si>
+    <t>Camilo</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>edad</t>
+  </si>
+  <si>
+    <t>genero</t>
+  </si>
+  <si>
+    <t>residencia</t>
+  </si>
+  <si>
+    <t>sisben</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Camila</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Urbano</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>Carla</t>
+  </si>
+  <si>
+    <t>Josefa</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Manuel</t>
+  </si>
+  <si>
+    <t>Carolina</t>
+  </si>
+  <si>
+    <t>Brayan</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Manuela</t>
+  </si>
+  <si>
+    <t>Joseline</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +109,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +131,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +435,275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregando 5 datos al excel y agregando los datos condicionales al excel
</commit_message>
<xml_diff>
--- a/Colegio.xlsx
+++ b/Colegio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26922394e5d0c289/Desktop/preParcial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4D2F04E46CFB4ACB3E209D9595F0AC683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A46FA276-EF18-466F-A269-AE8A32E0D6B3}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_AD4D2F04E46CFB4ACB3E209D9595F0AC683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FEE8250-067C-4D6E-B5C1-6E76C1EDD051}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
   <si>
     <t>Camilo</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>Joseline</t>
+  </si>
+  <si>
+    <t>Valentina</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Yuly</t>
+  </si>
+  <si>
+    <t>Yuri</t>
+  </si>
+  <si>
+    <t>Daniela</t>
   </si>
 </sst>
 </file>
@@ -436,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,6 +718,91 @@
         <v>5</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>